<commit_message>
Updated after LLP Feedback
</commit_message>
<xml_diff>
--- a/Config Files/AOC-4_nodes_seperated_config.xlsx
+++ b/Config Files/AOC-4_nodes_seperated_config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mns-admin\Documents\Python\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0E499C5-6C53-41F1-A3AC-B7C11B23657F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AD2C938-1534-4485-B9F4-C12DF9FD6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1455,8 +1455,8 @@
   <dimension ref="A1:L196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J121" sqref="J121"/>
+      <pane ySplit="1" topLeftCell="A170" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J180" sqref="J180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>